<commit_message>
[Kafka-consumer] 1) Added date header
</commit_message>
<xml_diff>
--- a/kafka-consumer-app/src/main/resources/templates/selgros_order_list_template.xlsx
+++ b/kafka-consumer-app/src/main/resources/templates/selgros_order_list_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PIS-2022L-KAFKA-PROD\kafka-consumer-app\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A4BB3E-25AD-4367-A776-C0776419E2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C7B9BC-B508-415F-B1E8-76F1117A6915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>SELGROS</t>
   </si>
@@ -77,39 +77,6 @@
   </si>
   <si>
     <t>Received At</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2022-05-28</t>
-  </si>
-  <si>
-    <t>Plac DUPA</t>
-  </si>
-  <si>
-    <t>tyototototodd</t>
-  </si>
-  <si>
-    <t>00-661</t>
-  </si>
-  <si>
-    <t>PL</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>2022-05-31</t>
   </si>
 </sst>
 </file>
@@ -414,10 +381,10 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="172" formatCode="00\-000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="00\-000"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -491,12 +458,12 @@
   <autoFilter ref="B3:K171" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Purcharser's code"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="EAN" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="EAN" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{6DDD753C-A844-49AA-BC69-580A07021138}" name="Quantity"/>
     <tableColumn id="14" xr3:uid="{5A48E342-F507-40F6-AAD4-3F597FF61D8C}" name="Received At"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Street"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="City"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Postal Code" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Postal Code" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Country Code"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Telephone Number"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Remarks"/>
@@ -804,7 +771,7 @@
   <dimension ref="A1:K171"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -877,388 +844,148 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="15">
-        <v>6</v>
-      </c>
-      <c r="C4" s="16">
-        <v>1</v>
-      </c>
-      <c r="D4" s="15">
-        <v>1000</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="15">
-        <v>48500500500</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="17">
-        <v>6</v>
-      </c>
-      <c r="C5" s="18">
-        <v>2</v>
-      </c>
-      <c r="D5" s="17">
-        <v>20</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="15">
-        <v>48500500500</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="15">
-        <v>6</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="15">
-        <v>30</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="15">
-        <v>48500500500</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="15">
-        <v>6</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="15">
-        <v>2</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="15">
-        <v>48500500500</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="15">
-        <v>7</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="15">
-        <v>60</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="15">
-        <v>48500500500</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="15">
-        <v>7</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="15">
-        <v>20</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="15">
-        <v>48500500500</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="15">
-        <v>7</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="15">
-        <v>30</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="15">
-        <v>48500500500</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="15">
-        <v>7</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="15">
-        <v>4</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="15">
-        <v>48500500500</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="15">
-        <v>6</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="15">
-        <v>70</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="15">
-        <v>48500500500</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
     </row>
     <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="15">
-        <v>6</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="15">
-        <v>20</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="15">
-        <v>48500500500</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="15">
-        <v>6</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="15">
-        <v>30</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="15">
-        <v>48500500500</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
     </row>
     <row r="15" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="15">
-        <v>6</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="15">
-        <v>40</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="15">
-        <v>48500500500</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
     </row>
     <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>

</xml_diff>